<commit_message>
Update test for correctly testing time value as string
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Initial Value</x:t>
   </x:si>
@@ -50,6 +50,9 @@
   </x:si>
   <x:si>
     <x:t>Test Case</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.02:31:45</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -579,11 +582,11 @@
       <x:c r="E7" s="5" t="n">
         <x:v>1.10538194444444</x:v>
       </x:c>
-      <x:c r="F7" s="5" t="n">
-        <x:v>1.10538194444444</x:v>
-      </x:c>
-      <x:c r="G7" s="5" t="n">
-        <x:v>1.10538194444444</x:v>
+      <x:c r="F7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Preserve whitespace in cells.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -7,6 +7,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Cell Values" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Test Whitespace" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
     <x:t>Initial Value</x:t>
   </x:si>
@@ -53,6 +54,9 @@
   </x:si>
   <x:si>
     <x:t>1.02:31:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">    </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -596,4 +600,29 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Load file's cached value into XLCell.CachedValue - need to some refactoring of the internal parsing in XLCell
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
     <x:t>Initial Value</x:t>
   </x:si>
@@ -54,6 +54,9 @@
   </x:si>
   <x:si>
     <x:t>1.02:31:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26:31:45</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">    </x:t>
@@ -465,7 +468,7 @@
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="12.270625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.920625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="9.830625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.250625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="19.660625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="21.270625" style="0" customWidth="1"/>
@@ -589,7 +592,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -614,7 +617,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Set IXLCell.Style.IncludeQuotePrefix to true if user sets IXLCell.Value to something that starts with single quote (in line with Excel)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -120,7 +120,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="6">
+  <x:cellStyleXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -133,6 +133,9 @@
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -140,7 +143,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -154,6 +157,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -508,10 +515,10 @@
       <x:c r="E3" s="3">
         <x:v>40423</x:v>
       </x:c>
-      <x:c r="F3" s="0" t="s">
+      <x:c r="F3" s="4" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
+      <x:c r="G3" s="4" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
@@ -528,15 +535,15 @@
       <x:c r="E4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="F4" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="s">
+      <x:c r="G4" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
-      <x:c r="B5" s="4" t="n">
+      <x:c r="B5" s="5" t="n">
         <x:v>1234.567</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
@@ -548,10 +555,10 @@
       <x:c r="E5" s="0" t="n">
         <x:v>1234.567</x:v>
       </x:c>
-      <x:c r="F5" s="0" t="s">
+      <x:c r="F5" s="4" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="G5" s="0" t="s">
+      <x:c r="G5" s="4" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
@@ -576,22 +583,22 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
-      <x:c r="B7" s="5" t="n">
+      <x:c r="B7" s="6" t="n">
         <x:v>1.10538194444444</x:v>
       </x:c>
-      <x:c r="C7" s="5" t="n">
+      <x:c r="C7" s="6" t="n">
         <x:v>1.10538194444444</x:v>
       </x:c>
-      <x:c r="D7" s="5" t="n">
+      <x:c r="D7" s="6" t="n">
         <x:v>1.10538194444444</x:v>
       </x:c>
-      <x:c r="E7" s="5" t="n">
+      <x:c r="E7" s="6" t="n">
         <x:v>1.10538194444444</x:v>
       </x:c>
-      <x:c r="F7" s="0" t="s">
+      <x:c r="F7" s="4" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="G7" s="0" t="s">
+      <x:c r="G7" s="4" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
@@ -616,7 +623,7 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:1">
-      <x:c r="A1" s="0" t="s">
+      <x:c r="A1" s="4" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>

</xml_diff>